<commit_message>
BCC ve Monsarj toplama kartlarının linkleri toplama kartları dosyasına eklendi.
</commit_message>
<xml_diff>
--- a/pages/toplama-kartlari.xlsx
+++ b/pages/toplama-kartlari.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>Sıra</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>CC-BCC-16-000-COP-P2B1-01</t>
-  </si>
-  <si>
     <t>BCC</t>
   </si>
   <si>
@@ -141,13 +138,22 @@
   </si>
   <si>
     <t>Model-01</t>
+  </si>
+  <si>
+    <t>CC-BCC-16-000-COP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/CC-BCC-16-000-COP-S2B1-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/CC-MNS-06-000-LOP-S2B1-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -186,6 +192,14 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -219,8 +233,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -239,17 +254,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,23 +615,23 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="49.6640625" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="4.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="52.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -658,64 +674,66 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" s="5"/>
     </row>
@@ -724,31 +742,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="5"/>
     </row>
@@ -757,31 +775,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -790,31 +808,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" s="5"/>
     </row>
@@ -823,70 +841,75 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="J7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>